<commit_message>
updated w new dat
</commit_message>
<xml_diff>
--- a/data/Daten_Distanz_Reisezeit_2022_korrigiert.xlsx
+++ b/data/Daten_Distanz_Reisezeit_2022_korrigiert.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kruegeto\Documents\eids\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE53D156-93A0-4C4D-838A-2DDF366CB5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441366B3-8280-418A-9373-C50C6FA78962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daten_Distanz_Reisezeit_2022" sheetId="1" r:id="rId1"/>
@@ -889,15 +889,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -908,7 +908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>60</v>
       </c>
@@ -918,12 +918,8 @@
       <c r="C2">
         <v>21</v>
       </c>
-      <c r="D2">
-        <f>A2-B2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>15</v>
       </c>
@@ -934,7 +930,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>57</v>
       </c>
@@ -945,7 +941,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>35</v>
       </c>
@@ -956,7 +952,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>38</v>
       </c>
@@ -967,7 +963,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>55</v>
       </c>
@@ -978,7 +974,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>45</v>
       </c>
@@ -989,7 +985,7 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>63</v>
       </c>
@@ -1000,7 +996,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>41</v>
       </c>
@@ -1011,7 +1007,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>60</v>
       </c>
@@ -1022,7 +1018,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>46</v>
       </c>
@@ -1033,7 +1029,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>81</v>
       </c>
@@ -1044,7 +1040,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
         <v>1.2</v>
       </c>
@@ -1055,7 +1051,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>56</v>
       </c>
@@ -1066,7 +1062,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>58</v>
       </c>
@@ -1077,7 +1073,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>57</v>
       </c>
@@ -1088,7 +1084,7 @@
         <v>10.42</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>13</v>
       </c>
@@ -1099,7 +1095,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>67</v>
       </c>
@@ -1110,7 +1106,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>30</v>
       </c>
@@ -1121,7 +1117,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>60</v>
       </c>
@@ -1132,7 +1128,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>58</v>
       </c>
@@ -1143,7 +1139,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>54</v>
       </c>
@@ -1154,7 +1150,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>45</v>
       </c>
@@ -1165,7 +1161,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>64</v>
       </c>
@@ -1176,7 +1172,7 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>75</v>
       </c>
@@ -1187,7 +1183,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>62</v>
       </c>
@@ -1198,7 +1194,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>40</v>
       </c>
@@ -1209,7 +1205,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>70</v>
       </c>
@@ -1220,7 +1216,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>70</v>
       </c>
@@ -1231,7 +1227,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>93</v>
       </c>
@@ -1242,7 +1238,7 @@
         <v>38.799999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>43</v>
       </c>
@@ -1253,7 +1249,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>44</v>
       </c>
@@ -1264,7 +1260,7 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>47</v>
       </c>
@@ -1275,7 +1271,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>53</v>
       </c>
@@ -1286,7 +1282,7 @@
         <v>12.17</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>48</v>
       </c>
@@ -1297,7 +1293,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>29</v>
       </c>
@@ -1308,7 +1304,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <v>121</v>
       </c>
@@ -1319,7 +1315,7 @@
         <v>74.099999999999994</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <v>55</v>
       </c>
@@ -1330,7 +1326,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1">
         <v>47</v>
       </c>
@@ -1341,7 +1337,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>81</v>
       </c>
@@ -1352,7 +1348,7 @@
         <v>27.37</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1363,7 +1359,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <v>28</v>
       </c>
@@ -1374,7 +1370,7 @@
         <v>3.34</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>20</v>
       </c>
@@ -1385,7 +1381,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <v>59</v>
       </c>
@@ -1396,7 +1392,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <v>10</v>
       </c>
@@ -1407,7 +1403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
         <v>47</v>
       </c>
@@ -1418,7 +1414,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <v>57</v>
       </c>
@@ -1429,7 +1425,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
         <v>50</v>
       </c>
@@ -1440,7 +1436,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <v>68</v>
       </c>
@@ -1451,7 +1447,7 @@
         <v>21.8</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
         <v>25</v>
       </c>
@@ -1462,7 +1458,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1473,7 +1469,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
         <v>59</v>
       </c>
@@ -1484,7 +1480,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
         <v>72</v>
       </c>
@@ -1495,7 +1491,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
         <v>67</v>
       </c>
@@ -1506,7 +1502,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
         <v>48</v>
       </c>
@@ -1517,7 +1513,7 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
         <v>50</v>
       </c>
@@ -1528,7 +1524,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
         <v>42</v>
       </c>
@@ -1539,7 +1535,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A59">
         <v>50</v>
       </c>
@@ -1550,7 +1546,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A60">
         <v>26</v>
       </c>
@@ -1561,7 +1557,7 @@
         <v>2.91</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A61">
         <v>19</v>
       </c>
@@ -1572,7 +1568,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
         <v>56</v>
       </c>
@@ -1583,7 +1579,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
         <v>56</v>
       </c>
@@ -1594,7 +1590,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
         <v>87</v>
       </c>
@@ -1605,7 +1601,7 @@
         <v>52.2</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
         <v>89</v>
       </c>
@@ -1616,7 +1612,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A66">
         <v>50</v>
       </c>
@@ -1627,7 +1623,7 @@
         <v>16.25</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A67">
         <v>85</v>
       </c>
@@ -1638,7 +1634,7 @@
         <v>28.85</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
         <v>37</v>
       </c>
@@ -1649,7 +1645,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
         <v>16</v>
       </c>
@@ -1660,7 +1656,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
         <v>55</v>
       </c>
@@ -1671,7 +1667,7 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1">
         <v>39</v>
       </c>
@@ -1682,7 +1678,7 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A72">
         <v>128</v>
       </c>
@@ -1693,7 +1689,7 @@
         <v>74.400000000000006</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A73">
         <v>74</v>
       </c>
@@ -1704,7 +1700,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A74">
         <v>19</v>
       </c>
@@ -1715,7 +1711,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A75">
         <v>45</v>
       </c>
@@ -1726,7 +1722,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A76">
         <v>60</v>
       </c>
@@ -1737,7 +1733,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A77">
         <v>39</v>
       </c>
@@ -1748,7 +1744,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A78">
         <v>110</v>
       </c>

</xml_diff>